<commit_message>
wip: updated excel file
</commit_message>
<xml_diff>
--- a/notes - doors quote generator.xlsx
+++ b/notes - doors quote generator.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>v 0.1</t>
   </si>
@@ -152,8 +152,22 @@
     <t>Will have to perfect the tool and sales material before I can market</t>
   </si>
   <si>
+    <t>New chrome API's will need to learn</t>
+  </si>
+  <si>
+    <t>Is not an ExpressJS app</t>
+  </si>
+  <si>
+    <t>vastly different code and folder structure</t>
+  </si>
+  <si>
+    <t>Y move to make product in a new domain before you even know the old one well enough</t>
+  </si>
+  <si>
     <t>Q: Which project do you want to do first???
-Ans: For my short term and long term, although my developer rating is 1/100, but for a saas product business, lifestyle and future, need to get started with developing, marketing and monetizing saas products, will be better prepared to launch the next saas product, need to figure out how to create a useful saas product and make money through it</t>
+Ans: For my short term and long term, although my developer rating is 1/100, but for a saas product business, lifestyle and future, need to get started with developing, marketing and monetizing saas products, will be better prepared to launch the next saas product, need to figure out how to create a useful saas product and make money through it
+Ans 2: For a competent developer, making a chrome plugin will not be a big deal after making something like the door quote automator, next step in the staicase is to up your skills, then can work on any idea you want, so level up skills by building the door quote automator.
+Ans 3: Any major decision will only be taken if tech is making $4000/month, this will require major upgradation of skills and will be a long journey, every project should be of such a high quality that it can also be showcased, even if you want to launch a saas product. Prudence demands that I am through in every project and focus on upgradation of skills, individual projects do not take more than 3-4 months, main objective should be constant improvement in skills and portfolio.</t>
   </si>
 </sst>
 </file>
@@ -335,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -371,21 +385,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -407,6 +408,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -920,31 +937,31 @@
       <c r="B1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="41" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="19" t="s">
@@ -955,142 +972,142 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="I5" s="23" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="I5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="I6" s="24" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="I6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>4</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="I7" s="25" t="s">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="I7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="I8" s="25" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="I8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="I9" s="24" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="I9" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>7</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="41" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1098,93 +1115,93 @@
       <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>2</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
         <v>3</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <v>4</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
         <v>5</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="20">
         <v>6</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <v>7</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1223,15 +1240,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="0.5703125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="0.5703125" style="23" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="9.140625" style="17"/>
@@ -1240,176 +1257,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="26" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="29" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="29" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="36"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="E7" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="D8" s="35" t="s">
+      <c r="B8" s="29"/>
+      <c r="D8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="36" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="D9" s="39" t="s">
+      <c r="B9" s="29"/>
+      <c r="D9" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="D10" s="39" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="D10" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="36"/>
-    </row>
-    <row r="11" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-    </row>
-    <row r="12" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+    </row>
+    <row r="12" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="36"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>